<commit_message>
feet:going to eat dinner
</commit_message>
<xml_diff>
--- a/06-03-2023/data/output/xlsx/Causality for Category/10.xlsx
+++ b/06-03-2023/data/output/xlsx/Causality for Category/10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="147">
   <si>
     <t>Causality Values Chart</t>
   </si>
@@ -52,39 +52,36 @@
     <t>num_of_adds_and_subs__1</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
+    <t>num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
   </si>
   <si>
     <t>num_of_adds_and_subs__2</t>
   </si>
   <si>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__3</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__4</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__5</t>
+  </si>
+  <si>
     <t>n/a</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__3</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__4</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__5</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
-  </si>
-  <si>
     <t>num_of_adds_and_subs__6</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
-  </si>
-  <si>
     <t>num_of_adds_and_subs__7</t>
   </si>
   <si>
@@ -127,30 +124,51 @@
     <t>num_of_decimals__1</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
   </si>
   <si>
     <t>num_of_decimals__2</t>
   </si>
   <si>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
     <t>num_of_decimals__3</t>
   </si>
   <si>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
     <t>num_of_decimals__4</t>
   </si>
   <si>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
     <t>num_of_decimals__5</t>
   </si>
   <si>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
     <t>num_of_decimals__6</t>
   </si>
   <si>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
     <t>num_of_decimals__7</t>
   </si>
   <si>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
     <t>num_of_decimals__8</t>
   </si>
   <si>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
     <t>num_of_decimals__9</t>
   </si>
   <si>
@@ -220,42 +238,39 @@
     <t>num_of_equals__1</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
   </si>
   <si>
     <t>num_of_equals__2</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
   </si>
   <si>
     <t>num_of_equals__3</t>
   </si>
   <si>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
     <t>num_of_equals__4</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__5,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
   </si>
   <si>
     <t>num_of_equals__5</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
   </si>
   <si>
     <t>num_of_equals__6</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
-  </si>
-  <si>
     <t>num_of_equals__7</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
-  </si>
-  <si>
     <t>num_of_equals__8</t>
   </si>
   <si>
@@ -325,15 +340,9 @@
     <t>num_of_unknowns__2</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
-  </si>
-  <si>
     <t>num_of_unknowns__3</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,pairs_of_parentheses__1,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
-  </si>
-  <si>
     <t>num_of_unknowns__4</t>
   </si>
   <si>
@@ -367,19 +376,16 @@
     <t>pairs_of_parentheses__1</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__2,pairs_of_parentheses__3</t>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__2</t>
   </si>
   <si>
     <t>pairs_of_parentheses__2</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__3</t>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__1,num_of_decimals__2,num_of_decimals__3,num_of_decimals__4,num_of_decimals__5,num_of_decimals__6,num_of_decimals__7,num_of_decimals__8,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,pairs_of_parentheses__1</t>
   </si>
   <si>
     <t>pairs_of_parentheses__3</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_adds_and_subs__6,num_of_decimals__1,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_equals__7,num_of_unknowns__2,num_of_unknowns__3,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
   </si>
   <si>
     <t>pairs_of_parentheses__4</t>
@@ -571,10 +577,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>AddsSubs!$C$4:$C$11</c:f>
+              <c:f>AddsSubs!$C$4:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -587,23 +593,17 @@
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>AddsSubs!$D$4:$D$11</c:f>
+              <c:f>AddsSubs!$D$4:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.002042900919305414</c:v>
+                  <c:v>0.001021450459652707</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.001210653753026634</c:v>
@@ -613,12 +613,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.005050505050505051</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.009523809523809525</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.01265822784810127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -675,7 +669,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
-                  <a:t>Probability of total failure</a:t>
+                  <a:t>Probability of getting into category 10</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -807,7 +801,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
-                  <a:t>Probability of total failure</a:t>
+                  <a:t>Probability of getting into category 10</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -871,10 +865,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Equations!$C$4:$C$12</c:f>
+              <c:f>Equations!$C$4:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -890,26 +884,20 @@
                 <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Equations!$D$4:$D$12</c:f>
+              <c:f>Equations!$D$4:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.002006018054162487</c:v>
+                  <c:v>0.001003009027081244</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.002018163471241171</c:v>
+                  <c:v>0.001009081735620585</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.001855287569573284</c:v>
@@ -919,12 +907,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.004901960784313725</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.007352941176470588</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0108695652173913</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -981,7 +963,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
-                  <a:t>Probability of total failure</a:t>
+                  <a:t>Probability of getting into category 10</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1045,24 +1027,66 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Decimals!$C$4:$C$6</c:f>
+              <c:f>Decimals!$C$4:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Decimals!$D$4:$D$6</c:f>
+              <c:f>Decimals!$D$4:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.003215434083601286</c:v>
+                  <c:v>0.001607717041800643</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.002032520325203252</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00273972602739726</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.003952569169960474</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.005988023952095809</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.007936507936507936</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.01176470588235294</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.01538461538461539</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1119,7 +1143,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
-                  <a:t>Probability of total failure</a:t>
+                  <a:t>Probability of getting into category 10</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1183,36 +1207,24 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Unknowns!$C$4:$C$8</c:f>
+              <c:f>Unknowns!$C$4:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Unknowns!$D$4:$D$8</c:f>
+              <c:f>Unknowns!$D$4:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.002004008016032064</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.002928257686676428</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.01052631578947368</c:v>
+                  <c:v>0.001002004008016032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1269,7 +1281,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
-                  <a:t>Probability of total failure</a:t>
+                  <a:t>Probability of getting into category 10</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1333,36 +1345,30 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>PairsOfParentheses!$C$4:$C$8</c:f>
+              <c:f>PairsOfParentheses!$C$4:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>PairsOfParentheses!$D$4:$D$8</c:f>
+              <c:f>PairsOfParentheses!$D$4:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.005025125628140704</c:v>
+                  <c:v>0.002512562814070352</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.006369426751592357</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.01333333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1419,7 +1425,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
-                  <a:t>Probability of total failure</a:t>
+                  <a:t>Probability of getting into category 10</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1985,16 +1991,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>0.002042900919305414</v>
+        <v>0.001021450459652707</v>
       </c>
       <c r="E3" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="1">
-        <v>0.006424025995841514</v>
+        <v>0.004576828254598964</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2011,11 +2017,13 @@
         <v>0.001210653753026634</v>
       </c>
       <c r="E4" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.00497548141407585</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2032,13 +2040,13 @@
         <v>0.003236245954692557</v>
       </c>
       <c r="E5" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="1">
-        <v>0.006707229902287241</v>
+        <v>0.007007188192036978</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2055,13 +2063,13 @@
         <v>0.005050505050505051</v>
       </c>
       <c r="E6" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="1">
-        <v>0.008715356258204852</v>
+        <v>0.00910787820124348</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2075,16 +2083,14 @@
         <v>5</v>
       </c>
       <c r="D7" s="1">
-        <v>0.009523809523809525</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.013156265208172</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2098,21 +2104,19 @@
         <v>6</v>
       </c>
       <c r="D8" s="1">
-        <v>0.01265822784810127</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.01607420618337894</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1">
         <v>52</v>
@@ -2124,16 +2128,16 @@
         <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1">
         <v>40</v>
@@ -2145,16 +2149,16 @@
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1">
         <v>22</v>
@@ -2166,16 +2170,16 @@
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1">
         <v>18</v>
@@ -2187,16 +2191,16 @@
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1">
         <v>10</v>
@@ -2208,16 +2212,16 @@
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1">
         <v>9</v>
@@ -2229,16 +2233,16 @@
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1">
         <v>8</v>
@@ -2250,16 +2254,16 @@
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1">
         <v>7</v>
@@ -2271,16 +2275,16 @@
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1">
         <v>6</v>
@@ -2292,16 +2296,16 @@
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1">
         <v>4</v>
@@ -2313,16 +2317,16 @@
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
@@ -2334,16 +2338,16 @@
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>2</v>
@@ -2355,16 +2359,16 @@
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1">
         <v>2</v>
@@ -2376,16 +2380,16 @@
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1">
         <v>622</v>
@@ -2394,21 +2398,21 @@
         <v>20</v>
       </c>
       <c r="D22" s="1">
-        <v>0.003215434083601286</v>
+        <v>0.001607717041800643</v>
       </c>
       <c r="E22" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G22" s="1">
-        <v>0.008164224676022885</v>
+        <v>0.005165655807173119</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1">
         <v>492</v>
@@ -2417,14 +2421,16 @@
         <v>21</v>
       </c>
       <c r="D23" s="1">
-        <v>0</v>
+        <v>0.002032520325203252</v>
       </c>
       <c r="E23" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1" t="s">
-        <v>12</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.00562667853902192</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2438,19 +2444,21 @@
         <v>22</v>
       </c>
       <c r="D24" s="1">
-        <v>0</v>
+        <v>0.00273972602739726</v>
       </c>
       <c r="E24" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1" t="s">
-        <v>12</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.006491784678425808</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1">
         <v>253</v>
@@ -2459,19 +2467,21 @@
         <v>23</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>0.003952569169960474</v>
       </c>
       <c r="E25" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1" t="s">
-        <v>12</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.007341856645189929</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1">
         <v>167</v>
@@ -2480,19 +2490,21 @@
         <v>24</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>0.005988023952095809</v>
       </c>
       <c r="E26" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1" t="s">
-        <v>12</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.00866338738202798</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1">
         <v>126</v>
@@ -2501,19 +2513,21 @@
         <v>25</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>0.007936507936507936</v>
       </c>
       <c r="E27" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1" t="s">
-        <v>12</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.01020780995244449</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1">
         <v>85</v>
@@ -2522,19 +2536,21 @@
         <v>26</v>
       </c>
       <c r="D28" s="1">
-        <v>0</v>
+        <v>0.01176470588235294</v>
       </c>
       <c r="E28" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1" t="s">
-        <v>12</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.01359782435631169</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1">
         <v>65</v>
@@ -2543,19 +2559,21 @@
         <v>27</v>
       </c>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>0.01538461538461539</v>
       </c>
       <c r="E29" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1" t="s">
-        <v>12</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.01720498538331941</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B30" s="1">
         <v>41</v>
@@ -2567,16 +2585,16 @@
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B31" s="1">
         <v>31</v>
@@ -2588,16 +2606,16 @@
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B32" s="1">
         <v>23</v>
@@ -2609,16 +2627,16 @@
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B33" s="1">
         <v>15</v>
@@ -2630,16 +2648,16 @@
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1">
         <v>10</v>
@@ -2651,16 +2669,16 @@
         <v>0</v>
       </c>
       <c r="E34" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B35" s="1">
         <v>7</v>
@@ -2672,16 +2690,16 @@
         <v>0</v>
       </c>
       <c r="E35" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B36" s="1">
         <v>6</v>
@@ -2693,16 +2711,16 @@
         <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B37" s="1">
         <v>6</v>
@@ -2714,16 +2732,16 @@
         <v>0</v>
       </c>
       <c r="E37" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B38" s="1">
         <v>5</v>
@@ -2735,16 +2753,16 @@
         <v>0</v>
       </c>
       <c r="E38" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B39" s="1">
         <v>4</v>
@@ -2756,16 +2774,16 @@
         <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B40" s="1">
         <v>4</v>
@@ -2777,16 +2795,16 @@
         <v>0</v>
       </c>
       <c r="E40" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B41" s="1">
         <v>3</v>
@@ -2798,16 +2816,16 @@
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B42" s="1">
         <v>2</v>
@@ -2819,16 +2837,16 @@
         <v>0</v>
       </c>
       <c r="E42" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B43" s="1">
         <v>2</v>
@@ -2840,16 +2858,16 @@
         <v>0</v>
       </c>
       <c r="E43" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B44" s="1">
         <v>2</v>
@@ -2861,16 +2879,16 @@
         <v>0</v>
       </c>
       <c r="E44" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B45" s="1">
         <v>2</v>
@@ -2882,16 +2900,16 @@
         <v>0</v>
       </c>
       <c r="E45" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B46" s="1">
         <v>1</v>
@@ -2903,16 +2921,16 @@
         <v>0</v>
       </c>
       <c r="E46" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
@@ -2924,16 +2942,16 @@
         <v>0</v>
       </c>
       <c r="E47" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B48" s="1">
         <v>1</v>
@@ -2945,16 +2963,16 @@
         <v>0</v>
       </c>
       <c r="E48" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B49" s="1">
         <v>1</v>
@@ -2966,16 +2984,16 @@
         <v>0</v>
       </c>
       <c r="E49" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
@@ -2987,16 +3005,16 @@
         <v>0</v>
       </c>
       <c r="E50" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B51" s="1">
         <v>1</v>
@@ -3008,16 +3026,16 @@
         <v>0</v>
       </c>
       <c r="E51" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B52" s="1">
         <v>997</v>
@@ -3026,21 +3044,21 @@
         <v>50</v>
       </c>
       <c r="D52" s="1">
-        <v>0.002006018054162487</v>
+        <v>0.001003009027081244</v>
       </c>
       <c r="E52" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G52" s="1">
-        <v>0.006380170772942585</v>
+        <v>0.004528417875117633</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B53" s="1">
         <v>991</v>
@@ -3049,21 +3067,21 @@
         <v>51</v>
       </c>
       <c r="D53" s="1">
-        <v>0.002018163471241171</v>
+        <v>0.001009081735620585</v>
       </c>
       <c r="E53" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="G53" s="1">
-        <v>0.006388187472066763</v>
+        <v>0.004535190863231353</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B54" s="1">
         <v>539</v>
@@ -3075,16 +3093,18 @@
         <v>0.001855287569573284</v>
       </c>
       <c r="E54" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1" t="s">
-        <v>12</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0.005034828826753237</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B55" s="1">
         <v>344</v>
@@ -3096,18 +3116,18 @@
         <v>0.002906976744186046</v>
       </c>
       <c r="E55" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="G55" s="1">
-        <v>0.006114980158626134</v>
+        <v>0.006008862499781394</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B56" s="1">
         <v>204</v>
@@ -3119,18 +3139,18 @@
         <v>0.004901960784313725</v>
       </c>
       <c r="E56" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="G56" s="1">
-        <v>0.007787722582611924</v>
+        <v>0.008895492409272867</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B57" s="1">
         <v>136</v>
@@ -3139,21 +3159,19 @@
         <v>55</v>
       </c>
       <c r="D57" s="1">
-        <v>0.007352941176470588</v>
+        <v>0</v>
       </c>
       <c r="E57" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G57" s="1">
-        <v>0.01048353303407479</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B58" s="1">
         <v>92</v>
@@ -3162,21 +3180,19 @@
         <v>56</v>
       </c>
       <c r="D58" s="1">
-        <v>0.0108695652173913</v>
+        <v>0</v>
       </c>
       <c r="E58" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G58" s="1">
-        <v>0.01422434007848596</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B59" s="1">
         <v>54</v>
@@ -3188,16 +3204,16 @@
         <v>0</v>
       </c>
       <c r="E59" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B60" s="1">
         <v>35</v>
@@ -3209,16 +3225,16 @@
         <v>0</v>
       </c>
       <c r="E60" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B61" s="1">
         <v>17</v>
@@ -3230,16 +3246,16 @@
         <v>0</v>
       </c>
       <c r="E61" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B62" s="1">
         <v>9</v>
@@ -3251,16 +3267,16 @@
         <v>0</v>
       </c>
       <c r="E62" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B63" s="1">
         <v>5</v>
@@ -3272,16 +3288,16 @@
         <v>0</v>
       </c>
       <c r="E63" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B64" s="1">
         <v>1</v>
@@ -3293,16 +3309,16 @@
         <v>0</v>
       </c>
       <c r="E64" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B65" s="1">
         <v>1</v>
@@ -3314,16 +3330,16 @@
         <v>0</v>
       </c>
       <c r="E65" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B66" s="1">
         <v>187</v>
@@ -3335,16 +3351,16 @@
         <v>0</v>
       </c>
       <c r="E66" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B67" s="1">
         <v>142</v>
@@ -3356,16 +3372,16 @@
         <v>0</v>
       </c>
       <c r="E67" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B68" s="1">
         <v>93</v>
@@ -3377,16 +3393,16 @@
         <v>0</v>
       </c>
       <c r="E68" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B69" s="1">
         <v>73</v>
@@ -3398,16 +3414,16 @@
         <v>0</v>
       </c>
       <c r="E69" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B70" s="1">
         <v>54</v>
@@ -3419,16 +3435,16 @@
         <v>0</v>
       </c>
       <c r="E70" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B71" s="1">
         <v>37</v>
@@ -3440,16 +3456,16 @@
         <v>0</v>
       </c>
       <c r="E71" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B72" s="1">
         <v>22</v>
@@ -3461,16 +3477,16 @@
         <v>0</v>
       </c>
       <c r="E72" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B73" s="1">
         <v>17</v>
@@ -3482,16 +3498,16 @@
         <v>0</v>
       </c>
       <c r="E73" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B74" s="1">
         <v>11</v>
@@ -3503,16 +3519,16 @@
         <v>0</v>
       </c>
       <c r="E74" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B75" s="1">
         <v>8</v>
@@ -3524,16 +3540,16 @@
         <v>0</v>
       </c>
       <c r="E75" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B76" s="1">
         <v>5</v>
@@ -3545,16 +3561,16 @@
         <v>0</v>
       </c>
       <c r="E76" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B77" s="1">
         <v>3</v>
@@ -3566,16 +3582,16 @@
         <v>0</v>
       </c>
       <c r="E77" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B78" s="1">
         <v>2</v>
@@ -3587,16 +3603,16 @@
         <v>0</v>
       </c>
       <c r="E78" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B79" s="1">
         <v>1</v>
@@ -3608,16 +3624,16 @@
         <v>0</v>
       </c>
       <c r="E79" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B80" s="1">
         <v>998</v>
@@ -3626,19 +3642,19 @@
         <v>78</v>
       </c>
       <c r="D80" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="E80" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B81" s="1">
         <v>683</v>
@@ -3647,21 +3663,19 @@
         <v>79</v>
       </c>
       <c r="D81" s="1">
-        <v>0.002928257686676428</v>
+        <v>0</v>
       </c>
       <c r="E81" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G81" s="1">
-        <v>0.008214453885459647</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B82" s="1">
         <v>95</v>
@@ -3670,21 +3684,19 @@
         <v>80</v>
       </c>
       <c r="D82" s="1">
-        <v>0.01052631578947368</v>
+        <v>0</v>
       </c>
       <c r="E82" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G82" s="1">
-        <v>0.01888616484408781</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B83" s="1">
         <v>52</v>
@@ -3696,16 +3708,16 @@
         <v>0</v>
       </c>
       <c r="E83" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B84" s="1">
         <v>23</v>
@@ -3717,16 +3729,16 @@
         <v>0</v>
       </c>
       <c r="E84" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B85" s="1">
         <v>14</v>
@@ -3738,16 +3750,16 @@
         <v>0</v>
       </c>
       <c r="E85" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B86" s="1">
         <v>11</v>
@@ -3759,16 +3771,16 @@
         <v>0</v>
       </c>
       <c r="E86" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B87" s="1">
         <v>7</v>
@@ -3780,16 +3792,16 @@
         <v>0</v>
       </c>
       <c r="E87" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B88" s="1">
         <v>5</v>
@@ -3801,16 +3813,16 @@
         <v>0</v>
       </c>
       <c r="E88" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B89" s="1">
         <v>3</v>
@@ -3822,16 +3834,16 @@
         <v>0</v>
       </c>
       <c r="E89" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B90" s="1">
         <v>2</v>
@@ -3843,16 +3855,16 @@
         <v>0</v>
       </c>
       <c r="E90" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B91" s="1">
         <v>1</v>
@@ -3864,16 +3876,16 @@
         <v>0</v>
       </c>
       <c r="E91" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B92" s="1">
         <v>1</v>
@@ -3885,16 +3897,16 @@
         <v>0</v>
       </c>
       <c r="E92" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B93" s="1">
         <v>398</v>
@@ -3903,21 +3915,21 @@
         <v>91</v>
       </c>
       <c r="D93" s="1">
-        <v>0.005025125628140704</v>
+        <v>0.002512562814070352</v>
       </c>
       <c r="E93" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G93" s="1">
-        <v>0.008226967561849555</v>
+        <v>0.00591863752032507</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B94" s="1">
         <v>157</v>
@@ -3929,18 +3941,18 @@
         <v>0.006369426751592357</v>
       </c>
       <c r="E94" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G94" s="1">
-        <v>0.01013503475010756</v>
+        <v>0.01114651556511993</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B95" s="1">
         <v>75</v>
@@ -3949,21 +3961,19 @@
         <v>93</v>
       </c>
       <c r="D95" s="1">
-        <v>0.01333333333333333</v>
+        <v>0</v>
       </c>
       <c r="E95" s="1">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G95" s="1">
-        <v>0.01764189495793798</v>
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B96" s="1">
         <v>43</v>
@@ -3975,16 +3985,16 @@
         <v>0</v>
       </c>
       <c r="E96" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="A97" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B97" s="1">
         <v>25</v>
@@ -3996,16 +4006,16 @@
         <v>0</v>
       </c>
       <c r="E97" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B98" s="1">
         <v>17</v>
@@ -4017,16 +4027,16 @@
         <v>0</v>
       </c>
       <c r="E98" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B99" s="1">
         <v>8</v>
@@ -4038,16 +4048,16 @@
         <v>0</v>
       </c>
       <c r="E99" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B100" s="1">
         <v>4</v>
@@ -4059,16 +4069,16 @@
         <v>0</v>
       </c>
       <c r="E100" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B101" s="1">
         <v>3</v>
@@ -4080,16 +4090,16 @@
         <v>0</v>
       </c>
       <c r="E101" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B102" s="1">
         <v>3</v>
@@ -4101,16 +4111,16 @@
         <v>0</v>
       </c>
       <c r="E102" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B103" s="1">
         <v>3</v>
@@ -4122,16 +4132,16 @@
         <v>0</v>
       </c>
       <c r="E103" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B104" s="1">
         <v>3</v>
@@ -4143,16 +4153,16 @@
         <v>0</v>
       </c>
       <c r="E104" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B105" s="1">
         <v>2</v>
@@ -4164,16 +4174,16 @@
         <v>0</v>
       </c>
       <c r="E105" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B106" s="1">
         <v>1</v>
@@ -4185,16 +4195,16 @@
         <v>0</v>
       </c>
       <c r="E106" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B107" s="1">
         <v>1</v>
@@ -4206,11 +4216,11 @@
         <v>0</v>
       </c>
       <c r="E107" s="1">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -4220,7 +4230,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4231,7 +4241,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -4254,25 +4264,25 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -4286,13 +4296,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="3">
-        <v>0.002042900919305414</v>
+        <v>0.001021450459652707</v>
       </c>
       <c r="E4" s="3">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F4" s="1">
-        <v>3.889290327334979E-05</v>
+        <v>1.944645163667489E-05</v>
       </c>
       <c r="G4" s="1">
         <f>1/(POWER(B4,1.5))</f>
@@ -4332,10 +4342,10 @@
         <v>0.001210653753026634</v>
       </c>
       <c r="E5" s="3">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F5" s="1">
-        <v>-0.0007933542630054295</v>
+        <v>0.0002086497450106025</v>
       </c>
       <c r="G5" s="1">
         <f>1/(POWER(B5,1.5))</f>
@@ -4375,10 +4385,10 @@
         <v>0.003236245954692557</v>
       </c>
       <c r="E6" s="3">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F6" s="1">
-        <v>0.001232237938660493</v>
+        <v>0.002234241946676525</v>
       </c>
       <c r="G6" s="1">
         <f>1/(POWER(B6,1.5))</f>
@@ -4418,10 +4428,10 @@
         <v>0.005050505050505051</v>
       </c>
       <c r="E7" s="3">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F7" s="1">
-        <v>0.003046497034472987</v>
+        <v>0.004048501042489019</v>
       </c>
       <c r="G7" s="1">
         <f>1/(POWER(B7,1.5))</f>
@@ -4444,92 +4454,6 @@
       </c>
       <c r="L7" s="1">
         <f>MIN(K7,1-D7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3">
-        <v>105</v>
-      </c>
-      <c r="C8" s="1">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.009523809523809525</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.00751980150777746</v>
-      </c>
-      <c r="G8" s="1">
-        <f>1/(POWER(B8,1.5))</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <f>SQRT((D8-POWER(10,-4))*B8*((1-D8+POWER(10,-4))*B8))</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <f>G8*H8</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
-        <v>1.95996398454</v>
-      </c>
-      <c r="K8" s="1">
-        <f>I8*J8</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="1">
-        <f>MIN(K8,1-D8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3">
-        <v>79</v>
-      </c>
-      <c r="C9" s="1">
-        <v>6</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.01265822784810127</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.0106542198320692</v>
-      </c>
-      <c r="G9" s="1">
-        <f>1/(POWER(B9,1.5))</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <f>SQRT((D9-POWER(10,-4))*B9*((1-D9+POWER(10,-4))*B9))</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <f>G9*H9</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1.95996398454</v>
-      </c>
-      <c r="K9" s="1">
-        <f>I9*J9</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="1">
-        <f>MIN(K9,1-D9)</f>
         <v>0</v>
       </c>
     </row>
@@ -4552,7 +4476,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -4575,25 +4499,25 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -4604,7 +4528,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4615,7 +4539,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -4638,30 +4562,30 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B4" s="3">
         <v>997</v>
@@ -4670,13 +4594,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="3">
-        <v>0.002006018054162487</v>
+        <v>0.001003009027081244</v>
       </c>
       <c r="E4" s="3">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F4" s="1">
-        <v>2.010038130423504E-06</v>
+        <v>1.005019065211752E-06</v>
       </c>
       <c r="G4" s="1">
         <f>1/(POWER(B4,1.5))</f>
@@ -4704,7 +4628,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B5" s="3">
         <v>991</v>
@@ -4713,13 +4637,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="3">
-        <v>0.002018163471241171</v>
+        <v>0.001009081735620585</v>
       </c>
       <c r="E5" s="3">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F5" s="1">
-        <v>1.415545520910659E-05</v>
+        <v>7.077727604553295E-06</v>
       </c>
       <c r="G5" s="1">
         <f>1/(POWER(B5,1.5))</f>
@@ -4747,7 +4671,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B6" s="3">
         <v>539</v>
@@ -4759,10 +4683,10 @@
         <v>0.001855287569573284</v>
       </c>
       <c r="E6" s="3">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F6" s="1">
-        <v>-0.0001487204464587801</v>
+        <v>0.0008532835615572519</v>
       </c>
       <c r="G6" s="1">
         <f>1/(POWER(B6,1.5))</f>
@@ -4790,7 +4714,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B7" s="3">
         <v>344</v>
@@ -4802,10 +4726,10 @@
         <v>0.002906976744186046</v>
       </c>
       <c r="E7" s="3">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F7" s="1">
-        <v>0.0009029687281539825</v>
+        <v>0.001904972736170014</v>
       </c>
       <c r="G7" s="1">
         <f>1/(POWER(B7,1.5))</f>
@@ -4833,7 +4757,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B8" s="3">
         <v>204</v>
@@ -4845,10 +4769,10 @@
         <v>0.004901960784313725</v>
       </c>
       <c r="E8" s="3">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F8" s="1">
-        <v>0.002897952768281661</v>
+        <v>0.003899956776297693</v>
       </c>
       <c r="G8" s="1">
         <f>1/(POWER(B8,1.5))</f>
@@ -4871,92 +4795,6 @@
       </c>
       <c r="L8" s="1">
         <f>MIN(K8,1-D8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="3">
-        <v>136</v>
-      </c>
-      <c r="C9" s="1">
-        <v>6</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.007352941176470588</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.005348933160438524</v>
-      </c>
-      <c r="G9" s="1">
-        <f>1/(POWER(B9,1.5))</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <f>SQRT((D9-POWER(10,-4))*B9*((1-D9+POWER(10,-4))*B9))</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <f>G9*H9</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1.95996398454</v>
-      </c>
-      <c r="K9" s="1">
-        <f>I9*J9</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="1">
-        <f>MIN(K9,1-D9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="3">
-        <v>92</v>
-      </c>
-      <c r="C10" s="1">
-        <v>7</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.0108695652173913</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.00886555720135924</v>
-      </c>
-      <c r="G10" s="1">
-        <f>1/(POWER(B10,1.5))</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <f>SQRT((D10-POWER(10,-4))*B10*((1-D10+POWER(10,-4))*B10))</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <f>G10*H10</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>1.95996398454</v>
-      </c>
-      <c r="K10" s="1">
-        <f>I10*J10</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="1">
-        <f>MIN(K10,1-D10)</f>
         <v>0</v>
       </c>
     </row>
@@ -4967,6 +4805,413 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="80.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3">
+        <v>622</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.001607717041800643</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.0006057130337846111</v>
+      </c>
+      <c r="G4" s="1">
+        <f>1/(POWER(B4,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <f>SQRT((D4-POWER(10,-4))*B4*((1-D4+POWER(10,-4))*B4))</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <f>G4*H4</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K4" s="1">
+        <f>I4*J4</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <f>MIN(K4,1-D4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3">
+        <v>492</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.002032520325203252</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.00103051631718722</v>
+      </c>
+      <c r="G5" s="1">
+        <f>1/(POWER(B5,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <f>SQRT((D5-POWER(10,-4))*B5*((1-D5+POWER(10,-4))*B5))</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <f>G5*H5</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K5" s="1">
+        <f>I5*J5</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <f>MIN(K5,1-D5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="3">
+        <v>365</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.00273972602739726</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.001737722019381228</v>
+      </c>
+      <c r="G6" s="1">
+        <f>1/(POWER(B6,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <f>SQRT((D6-POWER(10,-4))*B6*((1-D6+POWER(10,-4))*B6))</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <f>G6*H6</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K6" s="1">
+        <f>I6*J6</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <f>MIN(K6,1-D6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3">
+        <v>253</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.003952569169960474</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.002950565161944442</v>
+      </c>
+      <c r="G7" s="1">
+        <f>1/(POWER(B7,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f>SQRT((D7-POWER(10,-4))*B7*((1-D7+POWER(10,-4))*B7))</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <f>G7*H7</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K7" s="1">
+        <f>I7*J7</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <f>MIN(K7,1-D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="3">
+        <v>167</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.005988023952095809</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.004986019944079777</v>
+      </c>
+      <c r="G8" s="1">
+        <f>1/(POWER(B8,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SQRT((D8-POWER(10,-4))*B8*((1-D8+POWER(10,-4))*B8))</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <f>G8*H8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K8" s="1">
+        <f>I8*J8</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <f>MIN(K8,1-D8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3">
+        <v>126</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.007936507936507936</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.006934503928491904</v>
+      </c>
+      <c r="G9" s="1">
+        <f>1/(POWER(B9,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f>SQRT((D9-POWER(10,-4))*B9*((1-D9+POWER(10,-4))*B9))</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <f>G9*H9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K9" s="1">
+        <f>I9*J9</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <f>MIN(K9,1-D9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="3">
+        <v>85</v>
+      </c>
+      <c r="C10" s="1">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.01176470588235294</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.01076270187433691</v>
+      </c>
+      <c r="G10" s="1">
+        <f>1/(POWER(B10,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f>SQRT((D10-POWER(10,-4))*B10*((1-D10+POWER(10,-4))*B10))</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <f>G10*H10</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K10" s="1">
+        <f>I10*J10</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <f>MIN(K10,1-D10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3">
+        <v>65</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.01538461538461539</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.001002004008016032</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.01438261137659935</v>
+      </c>
+      <c r="G11" s="1">
+        <f>1/(POWER(B11,1.5))</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <f>SQRT((D11-POWER(10,-4))*B11*((1-D11+POWER(10,-4))*B11))</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <f>G11*H11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1.95996398454</v>
+      </c>
+      <c r="K11" s="1">
+        <f>I11*J11</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <f>MIN(K11,1-D11)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -4979,7 +5224,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -5002,45 +5247,45 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="B4" s="3">
-        <v>622</v>
+        <v>998</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="3">
-        <v>0.003215434083601286</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="E4" s="3">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F4" s="1">
-        <v>0.001211426067569222</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
         <f>1/(POWER(B4,1.5))</f>
@@ -5072,9 +5317,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5085,7 +5330,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -5108,45 +5353,45 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="B4" s="3">
-        <v>998</v>
+        <v>398</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="3">
-        <v>0.002004008016032064</v>
+        <v>0.002512562814070352</v>
       </c>
       <c r="E4" s="3">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>0.00151055880605432</v>
       </c>
       <c r="G4" s="1">
         <f>1/(POWER(B4,1.5))</f>
@@ -5174,22 +5419,22 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="B5" s="3">
-        <v>683</v>
+        <v>157</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="3">
-        <v>0.002928257686676428</v>
+        <v>0.006369426751592357</v>
       </c>
       <c r="E5" s="3">
-        <v>0.002004008016032064</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="F5" s="1">
-        <v>0.0009242496706443636</v>
+        <v>0.005367422743576325</v>
       </c>
       <c r="G5" s="1">
         <f>1/(POWER(B5,1.5))</f>
@@ -5212,241 +5457,6 @@
       </c>
       <c r="L5" s="1">
         <f>MIN(K5,1-D5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="3">
-        <v>95</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.01052631578947368</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.00852230777344162</v>
-      </c>
-      <c r="G6" s="1">
-        <f>1/(POWER(B6,1.5))</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <f>SQRT((D6-POWER(10,-4))*B6*((1-D6+POWER(10,-4))*B6))</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <f>G6*H6</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>1.95996398454</v>
-      </c>
-      <c r="K6" s="1">
-        <f>I6*J6</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="1">
-        <f>MIN(K6,1-D6)</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="80.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="3">
-        <v>398</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.005025125628140704</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.00302111761210864</v>
-      </c>
-      <c r="G4" s="1">
-        <f>1/(POWER(B4,1.5))</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <f>SQRT((D4-POWER(10,-4))*B4*((1-D4+POWER(10,-4))*B4))</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <f>G4*H4</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>1.95996398454</v>
-      </c>
-      <c r="K4" s="1">
-        <f>I4*J4</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <f>MIN(K4,1-D4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5" s="3">
-        <v>157</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.006369426751592357</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.004365418735560293</v>
-      </c>
-      <c r="G5" s="1">
-        <f>1/(POWER(B5,1.5))</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <f>SQRT((D5-POWER(10,-4))*B5*((1-D5+POWER(10,-4))*B5))</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <f>G5*H5</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>1.95996398454</v>
-      </c>
-      <c r="K5" s="1">
-        <f>I5*J5</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
-        <f>MIN(K5,1-D5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="3">
-        <v>75</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.01333333333333333</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.002004008016032064</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.01132932531730127</v>
-      </c>
-      <c r="G6" s="1">
-        <f>1/(POWER(B6,1.5))</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <f>SQRT((D6-POWER(10,-4))*B6*((1-D6+POWER(10,-4))*B6))</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <f>G6*H6</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>1.95996398454</v>
-      </c>
-      <c r="K6" s="1">
-        <f>I6*J6</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="1">
-        <f>MIN(K6,1-D6)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>